<commit_message>
test design form Login
</commit_message>
<xml_diff>
--- a/2.Test/testDesign_NhungnthPH08611.xlsx
+++ b/2.Test/testDesign_NhungnthPH08611.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -24,22 +25,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
-    <t>bbbbb</t>
-  </si>
-  <si>
-    <t>ccccc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+  <si>
+    <t>Requirement Level 1
+Yêu cầu cấp 1</t>
+  </si>
+  <si>
+    <t>Requirement Level 2
+Yêu cầu cấp 2</t>
+  </si>
+  <si>
+    <t>Requirement Level 3
+Yêu cầu cấp 3</t>
+  </si>
+  <si>
+    <t>TC_ID
+Mã TC</t>
+  </si>
+  <si>
+    <t>Test case description
+Mô tả TC</t>
+  </si>
+  <si>
+    <t>Test Type
+Kiểu TC</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>LOG_02</t>
+  </si>
+  <si>
+    <t>Not success</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>LOG_01</t>
+  </si>
+  <si>
+    <t>Check GUI Login</t>
+  </si>
+  <si>
+    <t>"Dựa vào hình ảnh 
+ +Label tiêu đề: 'Đăng nhập'. -Font:18px Mã màu:FFFFFF, Font Style:Arial
+ +Label :'Tên đăng nhập', 'Mật khẩu':Font:14px ,Mã màu :D3D3D3, Font Style:Arial
+ +Label:'Quên mật khẩu','Tạo tài khoản':Font:14px, Mã màu:778899,Font Style:Arial
+ +TextField tên đăng nhập (txt_tendangnhap): fontsize: 16px - color: white (#FFFFFF) - font style: Arial
+ +TextField Mật khẩu (txt_matkhau): fontsize: 16px - color: white (#FFFFFF) - font style: Arial
+ + Button Đăng nhập (btn_dangnhap): ""Đăng nhập"" - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080
+ + Button Thoát (btn_thoat): ""Thoát"" - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080
+ +Background color:FF69B4"</t>
+  </si>
+  <si>
+    <t>check Function Login</t>
+  </si>
+  <si>
+    <t>LOG_01.1</t>
+  </si>
+  <si>
+    <t>LOG_01.2</t>
+  </si>
+  <si>
+    <t>LOG_01.3</t>
+  </si>
+  <si>
+    <t>LOG_01.4</t>
+  </si>
+  <si>
+    <t>LOG_01.5</t>
+  </si>
+  <si>
+    <t>LOG_01.6</t>
+  </si>
+  <si>
+    <t>LOG_01.7</t>
+  </si>
+  <si>
+    <t>Check đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>Check để trống tên tài khoản và mật khẩu</t>
+  </si>
+  <si>
+    <t>Check nhập tên tài khoản và không nhập mật khẩu</t>
+  </si>
+  <si>
+    <t>Check Không nhập tên tài khoản và nhập mật khẩu</t>
+  </si>
+  <si>
+    <t>Check nhập tên tài khoản đúng và mật khẩu sai</t>
+  </si>
+  <si>
+    <t>Check nhập tên tài khoản sai và mật khẩu đúng</t>
+  </si>
+  <si>
+    <t>Check nhập tên tài khoản sai và mật khẩu sai</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Click [Quên mật khẩu] link</t>
+  </si>
+  <si>
+    <t>LOG_02.1</t>
+  </si>
+  <si>
+    <t>LOG_02.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,16 +158,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -64,15 +213,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal_Template_ESTestPro_Test Case" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -350,30 +583,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="78" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="38.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="229.5">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test design - nhung
</commit_message>
<xml_diff>
--- a/2.Test/testDesign_NhungnthPH08611.xlsx
+++ b/2.Test/testDesign_NhungnthPH08611.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TGDD\Desktop\agile\Nhom3-pt14304-ud\Nhom3-pt14304-ud\2.Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="12920" windowHeight="11020" activeTab="1"/>
+    <workbookView xWindow="4185" yWindow="0" windowWidth="12915" windowHeight="11025"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Quản lý tài khoản" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Requirement Level 1
 Yêu cầu cấp 1</t>
@@ -58,9 +63,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>LOG_02</t>
-  </si>
-  <si>
     <t>Not success</t>
   </si>
   <si>
@@ -73,41 +75,9 @@
     <t>Check GUI Login</t>
   </si>
   <si>
-    <t>"Dựa vào hình ảnh 
- +Label tiêu đề: 'Đăng nhập'. -Font:18px Mã màu:FFFFFF, Font Style:Arial
- +Label :'Tên đăng nhập', 'Mật khẩu':Font:14px ,Mã màu :D3D3D3, Font Style:Arial
- +Label:'Quên mật khẩu','Tạo tài khoản':Font:14px, Mã màu:778899,Font Style:Arial
- +TextField tên đăng nhập (txt_tendangnhap): fontsize: 16px - color: white (#FFFFFF) - font style: Arial
- +TextField Mật khẩu (txt_matkhau): fontsize: 16px - color: white (#FFFFFF) - font style: Arial
- + Button Đăng nhập (btn_dangnhap): ""Đăng nhập"" - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080
- + Button Thoát (btn_thoat): ""Thoát"" - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080
- +Background color:FF69B4"</t>
-  </si>
-  <si>
     <t>check Function Login</t>
   </si>
   <si>
-    <t>LOG_01.1</t>
-  </si>
-  <si>
-    <t>LOG_01.2</t>
-  </si>
-  <si>
-    <t>LOG_01.3</t>
-  </si>
-  <si>
-    <t>LOG_01.4</t>
-  </si>
-  <si>
-    <t>LOG_01.5</t>
-  </si>
-  <si>
-    <t>LOG_01.6</t>
-  </si>
-  <si>
-    <t>LOG_01.7</t>
-  </si>
-  <si>
     <t>Check đăng nhập thành công</t>
   </si>
   <si>
@@ -127,18 +97,6 @@
   </si>
   <si>
     <t>Check nhập tên tài khoản sai và mật khẩu sai</t>
-  </si>
-  <si>
-    <t>Quên mật khẩu</t>
-  </si>
-  <si>
-    <t>Click [Quên mật khẩu] link</t>
-  </si>
-  <si>
-    <t>LOG_02.1</t>
-  </si>
-  <si>
-    <t>LOG_02.2</t>
   </si>
   <si>
     <t>Check GUI Quản lý tài khoản</t>
@@ -156,11 +114,154 @@
 Kích thước bảng:50x50cm.
  +Background color:FF69B4"</t>
   </si>
+  <si>
+    <t>Log_01.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Label tiêu đề: 'Đăng nhập'. -Font:18px Mã màu:FFFFFF, Font Style:Arial
+</t>
+  </si>
+  <si>
+    <t>Log_01.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Label :'Tên đăng nhập', 'Mật khẩu':Font:14px ,Mã màu :D3D3D3, Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_01.3</t>
+  </si>
+  <si>
+    <t>Label:'Quên mật khẩu','Tạo tài khoản':Font:14px, Mã màu:778899,Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_01.4</t>
+  </si>
+  <si>
+    <t>TextField tên đăng nhập (txt_tendangnhap): fontsize: 16px - color: white (#FFFFFF) - font style: Arial</t>
+  </si>
+  <si>
+    <t>Log_01.5</t>
+  </si>
+  <si>
+    <t>TextField Mật khẩu (txt_matkhau): fontsize: 16px - color: white (#FFFFFF) - font style: Arial</t>
+  </si>
+  <si>
+    <t>Log_01.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Button Đăng nhập (btn_dangnhap): ""Đăng nhập"" - fontsize: 14px ; color: white(#FFFFFF) ; font style: Arial ; button size: 10px 24px - button color: #008080</t>
+  </si>
+  <si>
+    <t>Log_01.7</t>
+  </si>
+  <si>
+    <t>Button Thoát (btn_thoat): ""Thoát"" ;fontsize: 14px ; color: white(#FFFFFF) ;  font style: Arial ;  button size: 10px 24px ; button color: #008080</t>
+  </si>
+  <si>
+    <t>Log_01.8</t>
+  </si>
+  <si>
+    <t>Background color:FF69B4"</t>
+  </si>
+  <si>
+    <t>Log_02.1</t>
+  </si>
+  <si>
+    <t>Log_02.2</t>
+  </si>
+  <si>
+    <t>Log_02.3</t>
+  </si>
+  <si>
+    <t>Log_02.4</t>
+  </si>
+  <si>
+    <t>Log_02.5</t>
+  </si>
+  <si>
+    <t>Log_02.6</t>
+  </si>
+  <si>
+    <t>Log_02.7</t>
+  </si>
+  <si>
+    <t>Check GUI Quên mật khẩu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quên mật khẩu 1 </t>
+  </si>
+  <si>
+    <t>Log_03.1</t>
+  </si>
+  <si>
+    <t>Label tiêu đề: 'Đổi mật khẩu'. -Font:18px Mã màu:000000, Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_03.2</t>
+  </si>
+  <si>
+    <t>Label :'Email' :Font:14px ,Mã màu :000000, Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_03.3</t>
+  </si>
+  <si>
+    <t>Button Xác nhận (btn_xacnhan): - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080</t>
+  </si>
+  <si>
+    <t>Log_03.4</t>
+  </si>
+  <si>
+    <t>TextField Email (txt_email): fontsize: 16px - color: white (#FFFFFF) - font style: Arial</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu 2</t>
+  </si>
+  <si>
+    <t>Log_03.5</t>
+  </si>
+  <si>
+    <t>Label :'Mật khẩu mới ' :Font:14px ,Mã màu :000000, Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_03.6</t>
+  </si>
+  <si>
+    <t>Label :'Xác nhận' :Font:14px ,Mã màu :000000, Font Style:Arial</t>
+  </si>
+  <si>
+    <t>Log_03.7</t>
+  </si>
+  <si>
+    <t>TextField Mật khẩu mới (txt_matkhaumoi): fontsize: 16px - color: white (#FFFFFF) - font style: Arial</t>
+  </si>
+  <si>
+    <t>Log_03.8</t>
+  </si>
+  <si>
+    <t>TextField Xác nhận (txt_xacnhan): fontsize: 16px - color: white (#FFFFFF) - font style: Arial</t>
+  </si>
+  <si>
+    <t>Log_03.9</t>
+  </si>
+  <si>
+    <t>Button Đổi mật khẩu (btn_doimatkhau): "Doimatkhau" - fontsize: 14px - color: white(#FFFFFF) - font style: Arial - button size: 10px 24px - button color: #008080</t>
+  </si>
+  <si>
+    <t>Log_03.10</t>
+  </si>
+  <si>
+    <t>Background color:FF69B4</t>
+  </si>
+  <si>
+    <t>Check chức năng Quên mật khẩu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -282,7 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,8 +410,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -586,7 +703,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,243 +711,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection sqref="A1:G12"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="38.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="150">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="38.25">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="25.5">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="25.5">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.5">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="25.5">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
+      <c r="F10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="F11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="F12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="F13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="3" t="s">
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="F14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="F15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="3" t="s">
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="F16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.5">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="25.5">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="30">
+      <c r="D24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30">
+      <c r="D25" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="D26" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
+      <c r="B27" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -842,20 +1141,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="48.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="65">
+    <row r="1" spans="1:7" ht="38.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -878,26 +1177,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="296" customHeight="1">
+    <row r="2" spans="1:7" ht="296.10000000000002" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="49" customHeight="1">
+    <row r="3" spans="1:7" ht="48.95" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -906,7 +1205,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="56" customHeight="1">
+    <row r="4" spans="1:7" ht="56.1" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -915,7 +1214,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="65.5" customHeight="1">
+    <row r="5" spans="1:7" ht="65.45" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8"/>

</xml_diff>